<commit_message>
Fixed open class time in female half-marathon
It was pointed out by Tom Fryers that the pace (seconds/km) for the female half-marathon was less than the pace for the female 20 km even though the half-marathon is slightly longer than 20 km. This has been corrected in this upload by changing the open class time for the female half-marathon in these three files.
</commit_message>
<xml_diff>
--- a/2020 Files/FemaleRoadStd2020.xlsx
+++ b/2020 Files/FemaleRoadStd2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alan Jones\Documents\AgeGrade\Age-Grade-Tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alan Jones\Documents\AgeGrade\Age-Grade-Tables\2020 Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CAB5F467-B576-42ED-981A-7DFA1DB06FF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC3CB308-D8EE-4F8D-9963-DFFA76C21611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="300" windowWidth="19905" windowHeight="15450" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6945" yWindow="1305" windowWidth="24105" windowHeight="13545" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AgeStdFactors" sheetId="2" r:id="rId1"/>
@@ -1016,8 +1016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V108"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="A108" sqref="A108"/>
+    <sheetView zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1230,7 +1230,7 @@
         <v>3689.9999999999995</v>
       </c>
       <c r="M4" s="1">
-        <v>3871</v>
+        <v>3898</v>
       </c>
       <c r="N4" s="1">
         <v>4639.9999999999991</v>
@@ -1298,7 +1298,7 @@
         <v>4.2708333333333327E-2</v>
       </c>
       <c r="M5" s="2">
-        <v>4.4803240740740741E-2</v>
+        <v>4.5115740740740741E-2</v>
       </c>
       <c r="N5" s="2">
         <v>5.3703703703703691E-2</v>
@@ -8030,8 +8030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V108"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="A108" sqref="A108"/>
+    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8242,7 +8242,7 @@
         <v>3689.9999999999995</v>
       </c>
       <c r="M4" s="1">
-        <v>3871</v>
+        <v>3898</v>
       </c>
       <c r="N4" s="1">
         <v>4640</v>
@@ -8310,7 +8310,7 @@
         <v>4.2708333333333327E-2</v>
       </c>
       <c r="M5" s="2">
-        <v>4.4803240740740741E-2</v>
+        <v>4.5115740740740741E-2</v>
       </c>
       <c r="N5" s="2">
         <v>5.3703703703703705E-2</v>
@@ -14916,8 +14916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:V108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="G104" sqref="G104"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15122,7 +15122,7 @@
         <v>3689.9999999999995</v>
       </c>
       <c r="M4" s="1">
-        <v>3871</v>
+        <v>3898</v>
       </c>
       <c r="N4" s="1">
         <v>4640</v>
@@ -15190,7 +15190,7 @@
         <v>4.2708333333333327E-2</v>
       </c>
       <c r="M5" s="2">
-        <v>4.4803240740740741E-2</v>
+        <v>4.5115740740740741E-2</v>
       </c>
       <c r="N5" s="2">
         <v>5.3703703703703705E-2</v>

</xml_diff>